<commit_message>
I sketched out a test plan, prepared templates for test cases, a checklist
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+  <si>
+    <t>Модуль</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Приоритет</t>
+  </si>
+  <si>
+    <t>Предусловие</t>
+  </si>
+  <si>
+    <t>Шаги</t>
+  </si>
+  <si>
+    <t>Ожидаемый результат</t>
+  </si>
+  <si>
+    <t>Комментарий</t>
+  </si>
+  <si>
+    <t>Процент покрытия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Неавтоматизировано   </t>
+  </si>
+  <si>
+    <t>Неавтоматизировано</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Неавтоматизировано </t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +75,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -45,15 +112,200 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,9 +321,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -109,12 +361,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +401,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -181,7 +433,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -331,12 +583,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.21875" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="31.77734375" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="5">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="17"/>
+      <c r="B14" s="11">
+        <v>13</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>